<commit_message>
Refactored creation of markup into several distinct steps by using visitor pattern
</commit_message>
<xml_diff>
--- a/test/unit/data/CreateMarkupFromExcel.xlsx
+++ b/test/unit/data/CreateMarkupFromExcel.xlsx
@@ -5,14 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="4" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="390" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="390" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Comment" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Date" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Number" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Formula" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Umlaute" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Token" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Date" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Number" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Formula" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Umlaute" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="date1" vbProcedure="false">Date!$A$2</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>Test converions of data types. Directly and as result of formulas.</t>
   </si>
@@ -55,6 +56,15 @@
   </si>
   <si>
     <t>Displays: 01.31.13</t>
+  </si>
+  <si>
+    <t>regular</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>end</t>
   </si>
   <si>
     <t>value</t>
@@ -242,7 +252,7 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A14" activeCellId="1" pane="topLeft" sqref="A1 A14"/>
+      <selection activeCell="A14" activeCellId="0" pane="topLeft" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -316,10 +326,55 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A2:B5"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A6" activeCellId="0" pane="topLeft" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.5" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.5" outlineLevel="0" r="3">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.5" outlineLevel="0" r="5">
+      <c r="A5" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B5" activeCellId="1" pane="topLeft" sqref="A1 B5"/>
+      <selection activeCell="B5" activeCellId="0" pane="topLeft" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.35"/>
@@ -332,13 +387,13 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.05" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.35" outlineLevel="0" r="2">
@@ -346,10 +401,10 @@
         <v>40939</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -363,7 +418,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -371,7 +426,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B3" activeCellId="1" pane="topLeft" sqref="A1 B3"/>
+      <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -383,13 +438,13 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.6" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.35" outlineLevel="0" r="2">
@@ -397,10 +452,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.35" outlineLevel="0" r="3">
@@ -408,10 +463,10 @@
         <v>1.2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.35" outlineLevel="0" r="4">
@@ -420,10 +475,10 @@
         <v>0.666666666666667</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.05" outlineLevel="0" r="5">
@@ -431,10 +486,10 @@
         <v>7.41821149125</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -448,7 +503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -456,7 +511,7 @@
   <dimension ref="A1:C65535"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A6" activeCellId="1" pane="topLeft" sqref="A1 A6"/>
+      <selection activeCell="A6" activeCellId="0" pane="topLeft" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -466,13 +521,13 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.6" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.35" outlineLevel="0" r="2">
@@ -481,10 +536,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.35" outlineLevel="0" r="3">
@@ -493,10 +548,10 @@
         <v>1.4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.35" outlineLevel="0" r="4">
@@ -505,10 +560,10 @@
         <v>AB</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.35" outlineLevel="0" r="5">
@@ -517,10 +572,10 @@
         <v>40940</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.35" outlineLevel="0" r="6"/>
@@ -536,14 +591,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -552,9 +607,9 @@
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.6" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.5" outlineLevel="0" r="1">
       <c r="A1" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add space between cells in markup
</commit_message>
<xml_diff>
--- a/test/unit/data/CreateMarkupFromExcel.xlsx
+++ b/test/unit/data/CreateMarkupFromExcel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="390" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="6" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="661" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Comment" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,7 @@
     <sheet name="Number" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Formula" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Umlaute" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="TwoCellsSepartedBySpace" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="date1" vbProcedure="false">Date!$A$2</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Test converions of data types. Directly and as result of formulas.</t>
   </si>
@@ -125,6 +126,12 @@
   </si>
   <si>
     <t>äöüÄÖÜ</t>
+  </si>
+  <si>
+    <t>cell1</t>
+  </si>
+  <si>
+    <t>cell2</t>
   </si>
 </sst>
 </file>
@@ -326,9 +333,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:B5"/>
+  <dimension ref="A2:B6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A6" activeCellId="0" pane="topLeft" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -355,6 +362,7 @@
         <v>12</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.35" outlineLevel="0" r="6"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -621,4 +629,39 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>